<commit_message>
Add flat energy distrubtion
</commit_message>
<xml_diff>
--- a/21-Spreads4Tests/QuadrupoleDoublet.xlsx
+++ b/21-Spreads4Tests/QuadrupoleDoublet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ken.long/KL-GIT/CCAP/02-LhARA/04-LhARAlinearOptics/21-Spreads4Tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56E4B9D4-F1C3-874E-9A86-3C1604D9D7BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78EEED0A-EA3C-5248-81E0-32E68A031EDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="640" windowWidth="17260" windowHeight="19000" xr2:uid="{008B2FEE-BD6E-8742-A59F-ADD463C42F77}"/>
+    <workbookView xWindow="5960" yWindow="640" windowWidth="26060" windowHeight="19000" xr2:uid="{008B2FEE-BD6E-8742-A59F-ADD463C42F77}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="43">
   <si>
     <t>p</t>
   </si>
@@ -56,12 +56,6 @@
     <t>Particle</t>
   </si>
   <si>
-    <t>Quad</t>
-  </si>
-  <si>
-    <t>Length</t>
-  </si>
-  <si>
     <t>m</t>
   </si>
   <si>
@@ -71,9 +65,6 @@
     <t>T/m</t>
   </si>
   <si>
-    <t>k</t>
-  </si>
-  <si>
     <r>
       <t>m</t>
     </r>
@@ -88,9 +79,6 @@
     </r>
   </si>
   <si>
-    <t>sqrt(k)</t>
-  </si>
-  <si>
     <r>
       <t>m</t>
     </r>
@@ -105,9 +93,6 @@
     </r>
   </si>
   <si>
-    <t>l*sqrt(k)</t>
-  </si>
-  <si>
     <t>R</t>
   </si>
   <si>
@@ -129,9 +114,6 @@
     <t>s/m</t>
   </si>
   <si>
-    <t>1/c*10^9</t>
-  </si>
-  <si>
     <t>K</t>
   </si>
   <si>
@@ -166,19 +148,317 @@
     <t>Focusing strength</t>
   </si>
   <si>
-    <t>f</t>
-  </si>
-  <si>
     <t>Gap</t>
   </si>
   <si>
     <t>f*</t>
   </si>
   <si>
-    <t>f-1</t>
-  </si>
-  <si>
-    <t>Doublet</t>
+    <r>
+      <t>f</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>-1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>f</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>k</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>sqrt(k</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>sqrt(k</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>k</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <t>Fquad</t>
+  </si>
+  <si>
+    <t>Dquad</t>
+  </si>
+  <si>
+    <r>
+      <t>l</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*sqrt(k</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>l</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*sqrt(k</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>l</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>l</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1/c*10</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>9</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>f</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>-1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>f</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>f*</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>-1</t>
+    </r>
+  </si>
+  <si>
+    <t>FD doublet</t>
+  </si>
+  <si>
+    <t>DF doublet</t>
+  </si>
+  <si>
+    <t>Difference</t>
   </si>
 </sst>
 </file>
@@ -237,7 +517,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -407,16 +687,52 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -455,7 +771,19 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -770,10 +1098,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{210C9CAF-347D-914C-A112-6F8981E6D7C0}">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -781,345 +1109,491 @@
     <col min="1" max="1" width="17.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="22"/>
-    </row>
-    <row r="2" spans="1:10" ht="20" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
-      <c r="B2" s="4" t="s">
+    <row r="1" spans="1:13" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="21"/>
+    </row>
+    <row r="2" spans="1:13" ht="20" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="5"/>
-      <c r="H2" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" s="12">
+      <c r="C2" s="11"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="4"/>
+      <c r="K2" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="11">
         <v>938.27208815999995</v>
       </c>
-      <c r="J2" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
-        <v>24</v>
+      <c r="M2" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>18</v>
       </c>
       <c r="B3" s="1">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="23">
+        <v>0.03</v>
+      </c>
+      <c r="F3" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="23">
+        <v>0.03</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" s="23">
+        <v>299792458</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="5"/>
+      <c r="B4" s="17"/>
+      <c r="D4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E3">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="F3" s="7" t="s">
+      <c r="E4" s="23">
+        <v>325</v>
+      </c>
+      <c r="F4" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" s="12">
-        <v>299792458</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="6"/>
-      <c r="B4" s="18"/>
-      <c r="D4" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4">
-        <v>500</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="I4">
-        <f>1/I3</f>
+      <c r="G4" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="23">
+        <v>325</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L4" s="23">
+        <f>1/L3</f>
         <v>3.3356409519815204E-9</v>
       </c>
-      <c r="J4" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+      <c r="M4" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="19" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="1">
-        <f>SQRT( (I2+B3)^2 - I2^2)</f>
-        <v>137.35152624998378</v>
+        <f>SQRT( (L2+B3)^2 - L2^2)</f>
+        <v>150.5407921987921</v>
       </c>
       <c r="C5" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="13"/>
-      <c r="F5" s="7"/>
-      <c r="H5" s="8" t="s">
+      <c r="D5" s="12"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="6"/>
+      <c r="K5" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="L5" s="8">
+        <f>L4*1000000000</f>
+        <v>3.3356409519815204</v>
+      </c>
+      <c r="M5" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="20" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="8">
+        <f>L5*B5/1000</f>
+        <v>0.50215003140203107</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="23">
+        <f>E4/B6</f>
+        <v>647.21692656790594</v>
+      </c>
+      <c r="F6" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="23">
+        <f>H4/B6</f>
+        <v>647.21692656790594</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="20" x14ac:dyDescent="0.25">
+      <c r="D7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="23">
+        <f>SQRT(E6)</f>
+        <v>25.44045845828856</v>
+      </c>
+      <c r="F7" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="23">
+        <f>SQRT(H6)</f>
+        <v>25.44045845828856</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="D8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="23">
+        <f>E7*E3</f>
+        <v>0.76321375374865674</v>
+      </c>
+      <c r="F8" s="23"/>
+      <c r="G8" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" s="23">
+        <f>H3*H7</f>
+        <v>0.76321375374865674</v>
+      </c>
+      <c r="I8" s="6"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D9" s="5"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="6"/>
+    </row>
+    <row r="10" spans="1:13" ht="20" x14ac:dyDescent="0.25">
+      <c r="D10" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="23">
+        <f>E6*E3</f>
+        <v>19.416507797037177</v>
+      </c>
+      <c r="F10" s="23"/>
+      <c r="G10" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="H10" s="23">
+        <f>H6*H3</f>
+        <v>19.416507797037177</v>
+      </c>
+      <c r="I10" s="6"/>
+    </row>
+    <row r="11" spans="1:13" ht="18" x14ac:dyDescent="0.25">
+      <c r="D11" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="23">
+        <f>1/E10</f>
+        <v>5.1502567323285238E-2</v>
+      </c>
+      <c r="F11" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="H11" s="23">
+        <f>1/H10</f>
+        <v>5.1502567323285238E-2</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D12" s="18"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="9"/>
+    </row>
+    <row r="14" spans="1:13" ht="21" x14ac:dyDescent="0.25">
+      <c r="D14" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="20"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="H14" s="20"/>
+      <c r="I14" s="21"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D15" s="10"/>
+      <c r="E15" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="24">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G15" s="24"/>
+      <c r="H15" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="I15" s="4"/>
+    </row>
+    <row r="16" spans="1:13" ht="19" x14ac:dyDescent="0.2">
+      <c r="D16" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="23">
+        <f>E10-H10+F15*(E10*H10)</f>
+        <v>1.8850038751620275</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="H16" s="23">
+        <f>-E10+H10+F15*(E10*H10)</f>
+        <v>1.8850038751620275</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D17" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="9">
-        <f>I4*1000000000</f>
-        <v>3.3356409519815204</v>
-      </c>
-      <c r="J5" s="10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="19" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="9">
-        <f>I5*B5/1000</f>
-        <v>0.4581553757766107</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="6" t="s">
+      <c r="E17" s="8">
+        <f>1/E16</f>
+        <v>0.5305028881779057</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17" s="8">
+        <f>1/H16</f>
+        <v>0.5305028881779057</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="2">
+        <f>1+($F$15/$E$11)</f>
+        <v>1.0970825389851859</v>
+      </c>
+      <c r="C19" s="11">
+        <f>$F$15</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D19" s="11">
+        <v>0</v>
+      </c>
+      <c r="E19" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B20" s="12">
+        <f>-$E$16</f>
+        <v>-1.8850038751620275</v>
+      </c>
+      <c r="C20" s="23">
+        <f>1+($F$15/$H$11)</f>
+        <v>1.0970825389851859</v>
+      </c>
+      <c r="D20" s="23">
+        <v>0</v>
+      </c>
+      <c r="E20" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B21" s="12">
+        <v>0</v>
+      </c>
+      <c r="C21" s="23">
+        <v>0</v>
+      </c>
+      <c r="D21" s="23">
+        <f>1-($F$15/$E$11)</f>
+        <v>0.90291746101481407</v>
+      </c>
+      <c r="E21" s="6">
+        <f>$F$15</f>
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B22" s="18">
+        <v>0</v>
+      </c>
+      <c r="C22" s="8">
+        <v>0</v>
+      </c>
+      <c r="D22" s="8">
+        <f>-$H$16</f>
+        <v>-1.8850038751620275</v>
+      </c>
+      <c r="E22" s="9">
+        <f>1-($F$15/$H$11)</f>
+        <v>0.90291746101481407</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E6">
-        <f>E4/B6</f>
-        <v>1091.3328238317824</v>
-      </c>
-      <c r="F6" s="7" t="s">
+      <c r="B24" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="D24" s="13" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="19" x14ac:dyDescent="0.2">
-      <c r="D7" s="6" t="s">
+      <c r="E24" s="14">
+        <f t="array" ref="E24:E27">MMULT(B19:E22,B24:B27)</f>
+        <v>0.54904126949259291</v>
+      </c>
+      <c r="G24" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E7">
-        <f>SQRT(E6)</f>
-        <v>33.035326906688582</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="D8" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8">
-        <f>E7*E3</f>
-        <v>0.59463588432039438</v>
-      </c>
-      <c r="F8" s="7"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="D9" s="6"/>
-      <c r="F9" s="7"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="D10" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10">
-        <f>E6*E3</f>
-        <v>19.643990828972083</v>
-      </c>
-      <c r="F10" s="7"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="D11" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11">
-        <f>1/E10</f>
-        <v>5.0906152864067862E-2</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="D12" s="19"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="10"/>
-    </row>
-    <row r="14" spans="1:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="D14" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="21"/>
-      <c r="F14" s="22"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="D15" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="E15" s="12">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="D16" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E16" s="9">
-        <f>1/B19</f>
-        <v>-0.51828727988396894</v>
-      </c>
-      <c r="F16" s="10"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" s="3">
-        <f>1+($E$15/$E$11)</f>
-        <v>1.0982199541448605</v>
-      </c>
-      <c r="C18" s="12">
-        <f>$E$15</f>
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="D18" s="12">
+      <c r="H24" s="14">
+        <f>B$24*B19+B$25*C19+B$26*D19+B$27*E19</f>
+        <v>0.54904126949259291</v>
+      </c>
+      <c r="J24" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="K24" s="26">
+        <f>E24-H24</f>
         <v>0</v>
       </c>
-      <c r="E18" s="5">
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B25" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="E25" s="15">
+        <v>-0.83279368368249518</v>
+      </c>
+      <c r="H25" s="15">
+        <f>B$24*B20+B$25*C20+B$26*D20+B$27*E20</f>
+        <v>-0.83279368368249518</v>
+      </c>
+      <c r="K25" s="27">
+        <f t="shared" ref="K25:K27" si="0">E25-H25</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B19" s="13">
-        <f>-$E$15/$E$11^2</f>
-        <v>-1.9294318784436963</v>
-      </c>
-      <c r="C19" s="23">
-        <f>1-($E$15/$E$11)</f>
-        <v>0.9017800458551396</v>
-      </c>
-      <c r="D19" s="23">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B26" s="15">
+        <v>-0.3</v>
+      </c>
+      <c r="E26" s="15">
+        <v>-0.27187523830444421</v>
+      </c>
+      <c r="H26" s="15">
+        <f>B$24*B21+B$25*C21+B$26*D21+B$27*E21</f>
+        <v>-0.27187523830444421</v>
+      </c>
+      <c r="K26" s="27">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E19" s="7">
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B27" s="16">
+        <v>-0.2</v>
+      </c>
+      <c r="E27" s="16">
+        <v>0.38491767034564545</v>
+      </c>
+      <c r="H27" s="16">
+        <f>B$24*B22+B$25*C22+B$26*D22+B$27*E22</f>
+        <v>0.38491767034564545</v>
+      </c>
+      <c r="K27" s="28">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B20" s="13">
-        <v>0</v>
-      </c>
-      <c r="C20" s="23">
-        <v>0</v>
-      </c>
-      <c r="D20" s="23">
-        <f>1+($E$15/$E$11)</f>
-        <v>1.0982199541448605</v>
-      </c>
-      <c r="E20" s="7">
-        <f>$E$15</f>
-        <v>5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B21" s="19">
-        <v>0</v>
-      </c>
-      <c r="C21" s="9">
-        <v>0</v>
-      </c>
-      <c r="D21" s="9">
-        <f>-$E$15/$E$11^2</f>
-        <v>-1.9294318784436963</v>
-      </c>
-      <c r="E21" s="10">
-        <f>1-($E$15/$E$11)</f>
-        <v>0.9017800458551396</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B23" s="15">
-        <v>0.5</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E23" s="15">
-        <f t="array" ref="E23:E26">MMULT(B18:E21,B23:B26)</f>
-        <v>0.5496099770724302</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H23" s="15">
-        <f>B$23*B18+B$24*C18+B$25*D18+B$26*E18</f>
-        <v>0.5496099770724302</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B24" s="16">
-        <v>0.1</v>
-      </c>
-      <c r="E24" s="16">
-        <v>-0.87453793463633422</v>
-      </c>
-      <c r="H24" s="16">
-        <f>B$23*B19+B$24*C19+B$25*D19+B$26*E19</f>
-        <v>-0.87453793463633422</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B25" s="16">
-        <v>-0.3</v>
-      </c>
-      <c r="E25" s="16">
-        <v>-0.33046598624345813</v>
-      </c>
-      <c r="H25" s="16">
-        <f>B$23*B20+B$24*C20+B$25*D20+B$26*E20</f>
-        <v>-0.33046598624345813</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B26" s="17">
-        <v>-0.2</v>
-      </c>
-      <c r="E26" s="17">
-        <v>0.39847355436208098</v>
-      </c>
-      <c r="H26" s="17">
-        <f>B$23*B21+B$24*C21+B$25*D21+B$26*E21</f>
-        <v>0.39847355436208098</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:F1"/>
+  <mergeCells count="4">
     <mergeCell ref="D14:F14"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="F15:G15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>